<commit_message>
excel for multiple product upload done
</commit_message>
<xml_diff>
--- a/src/assets/ExcelSampleFile/sampleFullData.xlsx
+++ b/src/assets/ExcelSampleFile/sampleFullData.xlsx
@@ -3,8 +3,8 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:mv="urn:schemas-microsoft-com:mac:vml" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
   <workbookPr/>
   <sheets>
-    <sheet state="visible" name="First" sheetId="1" r:id="rId4"/>
-    <sheet state="visible" name="Second" sheetId="2" r:id="rId5"/>
+    <sheet state="visible" name="FirstSheet" sheetId="1" r:id="rId4"/>
+    <sheet state="visible" name="SecondSheet" sheetId="2" r:id="rId5"/>
   </sheets>
   <definedNames/>
   <calcPr/>
@@ -12,166 +12,208 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="111" uniqueCount="51">
-  <si>
-    <t>Name</t>
-  </si>
-  <si>
-    <t>Price</t>
-  </si>
-  <si>
-    <t>Old Price</t>
-  </si>
-  <si>
-    <t>Image</t>
-  </si>
-  <si>
-    <t>Sizes</t>
-  </si>
-  <si>
-    <t>Colors</t>
-  </si>
-  <si>
-    <t>Description</t>
-  </si>
-  <si>
-    <t>Stock Quantity</t>
-  </si>
-  <si>
-    <t>Order Quantity</t>
-  </si>
-  <si>
-    <t>Product Code</t>
-  </si>
-  <si>
-    <t>Category</t>
-  </si>
-  <si>
-    <t>Sub Title</t>
-  </si>
-  <si>
-    <t>Brand</t>
-  </si>
-  <si>
-    <t>Weight</t>
-  </si>
-  <si>
-    <t>Composition</t>
-  </si>
-  <si>
-    <t>Tags</t>
-  </si>
-  <si>
-    <t>image1.jpg</t>
-  </si>
-  <si>
-    <t>L, XL</t>
-  </si>
-  <si>
-    <t>Red, Yellow, #ddd</t>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="109" uniqueCount="65">
+  <si>
+    <t>name</t>
+  </si>
+  <si>
+    <t>code</t>
+  </si>
+  <si>
+    <t>subTitle</t>
+  </si>
+  <si>
+    <t>description</t>
+  </si>
+  <si>
+    <t>price</t>
+  </si>
+  <si>
+    <t>costPrice</t>
+  </si>
+  <si>
+    <t>category</t>
+  </si>
+  <si>
+    <t>gender</t>
+  </si>
+  <si>
+    <t>brand</t>
+  </si>
+  <si>
+    <t>weight</t>
+  </si>
+  <si>
+    <t>composition</t>
+  </si>
+  <si>
+    <t>tags</t>
+  </si>
+  <si>
+    <t>orderQuantity</t>
+  </si>
+  <si>
+    <t>color</t>
+  </si>
+  <si>
+    <t>size:quantity</t>
+  </si>
+  <si>
+    <t>photo</t>
+  </si>
+  <si>
+    <t>Product 1</t>
+  </si>
+  <si>
+    <t>XYZ</t>
+  </si>
+  <si>
+    <t>Subtitle A</t>
   </si>
   <si>
     <t>This is product 1</t>
   </si>
   <si>
+    <t>Kurti</t>
+  </si>
+  <si>
+    <t>Female</t>
+  </si>
+  <si>
+    <t>Brand X</t>
+  </si>
+  <si>
+    <t>8 kg</t>
+  </si>
+  <si>
+    <t>100% Cotton</t>
+  </si>
+  <si>
+    <t>Tag1, Tag3</t>
+  </si>
+  <si>
     <t>7, 8, 1</t>
   </si>
   <si>
-    <t>CODE1</t>
-  </si>
-  <si>
-    <t>Category A</t>
-  </si>
-  <si>
-    <t>Subtitle A</t>
-  </si>
-  <si>
-    <t>Brand X</t>
-  </si>
-  <si>
-    <t>8 kg</t>
-  </si>
-  <si>
-    <t>100% Cotton</t>
-  </si>
-  <si>
-    <t>Tag1, Tag3</t>
-  </si>
-  <si>
-    <t>Product 33</t>
-  </si>
-  <si>
-    <t>image1.jpg, image2.jpg, image3.jpg</t>
-  </si>
-  <si>
-    <t>L, S</t>
-  </si>
-  <si>
-    <t>Green, Blue</t>
+    <t>#FF0000</t>
+  </si>
+  <si>
+    <t>X:23, L:40</t>
+  </si>
+  <si>
+    <t>link1, link2, link3</t>
+  </si>
+  <si>
+    <t>#f5cb42</t>
+  </si>
+  <si>
+    <t>XS:100, M:50, L:80</t>
+  </si>
+  <si>
+    <t>Product 2</t>
+  </si>
+  <si>
+    <t>ABC</t>
+  </si>
+  <si>
+    <t>Subtitle B</t>
   </si>
   <si>
     <t>This is product 2</t>
   </si>
   <si>
+    <t>Shirt</t>
+  </si>
+  <si>
+    <t>Brand Y</t>
+  </si>
+  <si>
+    <t>1 kg</t>
+  </si>
+  <si>
+    <t>Tag2, Tag4</t>
+  </si>
+  <si>
     <t>1, 4, 9</t>
   </si>
   <si>
-    <t>CODE2</t>
-  </si>
-  <si>
-    <t>Subtitle B</t>
-  </si>
-  <si>
-    <t>Brand Y</t>
-  </si>
-  <si>
-    <t>1 kg</t>
-  </si>
-  <si>
-    <t>Tag2, Tag4</t>
-  </si>
-  <si>
-    <t>M, L</t>
-  </si>
-  <si>
-    <t>Red, Yellow, #FFF</t>
+    <t>#00FF00</t>
+  </si>
+  <si>
+    <t>XS:60, M:50, L:20</t>
+  </si>
+  <si>
+    <t>link1, link2</t>
+  </si>
+  <si>
+    <t>Product 3</t>
+  </si>
+  <si>
+    <t>AYD</t>
   </si>
   <si>
     <t>This is product 3</t>
   </si>
   <si>
+    <t>T-shirt</t>
+  </si>
+  <si>
+    <t>Male</t>
+  </si>
+  <si>
+    <t>7 kg</t>
+  </si>
+  <si>
+    <t>Tag2, Tag3</t>
+  </si>
+  <si>
     <t>5, 6, 2</t>
   </si>
   <si>
-    <t>CODE3</t>
-  </si>
-  <si>
-    <t>7 kg</t>
-  </si>
-  <si>
-    <t>Tag2, Tag3</t>
-  </si>
-  <si>
-    <t>extra</t>
-  </si>
-  <si>
-    <t>Product 1</t>
-  </si>
-  <si>
-    <t>Product 2</t>
-  </si>
-  <si>
-    <t>Product 3</t>
-  </si>
-  <si>
-    <t>10 kg</t>
+    <t>#00FFFF</t>
+  </si>
+  <si>
+    <t>L:100, XL:45</t>
+  </si>
+  <si>
+    <t>link1, link2, link3, link4</t>
+  </si>
+  <si>
+    <t>#a83275</t>
+  </si>
+  <si>
+    <t>L:75, XS:60, XL:25</t>
+  </si>
+  <si>
+    <t>#c92926</t>
+  </si>
+  <si>
+    <t>M:40, L:60, XXL:70</t>
+  </si>
+  <si>
+    <t>Product 4</t>
+  </si>
+  <si>
+    <t>OKK</t>
+  </si>
+  <si>
+    <t>Subtitle K</t>
+  </si>
+  <si>
+    <t>This is product 4</t>
+  </si>
+  <si>
+    <t>Jeans</t>
+  </si>
+  <si>
+    <t>Brand OK</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-  <fonts count="3">
+  <fonts count="4">
     <font>
       <sz val="11.0"/>
       <color theme="1"/>
@@ -182,7 +224,10 @@
       <b/>
       <color theme="1"/>
       <name val="Calibri"/>
-      <scheme val="minor"/>
+    </font>
+    <font>
+      <color theme="1"/>
+      <name val="Calibri"/>
     </font>
     <font>
       <color theme="1"/>
@@ -208,12 +253,14 @@
     <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment readingOrder="0" shrinkToFit="0" vertical="bottom" wrapText="0"/>
     </xf>
-    <xf borderId="0" fillId="0" fontId="1" numFmtId="0" xfId="0" applyFont="1"/>
     <xf borderId="0" fillId="0" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment readingOrder="0"/>
     </xf>
     <xf borderId="0" fillId="0" fontId="2" numFmtId="0" xfId="0" applyFont="1"/>
     <xf borderId="0" fillId="0" fontId="2" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
+      <alignment readingOrder="0"/>
+    </xf>
+    <xf borderId="0" fillId="0" fontId="3" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment readingOrder="0"/>
     </xf>
   </cellXfs>
@@ -437,22 +484,24 @@
   <sheetFormatPr customHeight="1" defaultColWidth="14.43" defaultRowHeight="15.0"/>
   <cols>
     <col customWidth="1" min="1" max="1" width="13.14"/>
-    <col customWidth="1" min="2" max="2" width="14.86"/>
-    <col customWidth="1" min="3" max="3" width="10.0"/>
-    <col customWidth="1" min="4" max="4" width="33.57"/>
-    <col customWidth="1" min="5" max="5" width="11.29"/>
-    <col customWidth="1" min="6" max="6" width="16.0"/>
-    <col customWidth="1" min="7" max="7" width="20.14"/>
-    <col customWidth="1" min="8" max="8" width="14.86"/>
-    <col customWidth="1" min="9" max="9" width="13.71"/>
-    <col customWidth="1" min="10" max="10" width="16.0"/>
-    <col customWidth="1" min="11" max="11" width="15.0"/>
-    <col customWidth="1" min="12" max="12" width="21.29"/>
-    <col customWidth="1" min="13" max="13" width="13.86"/>
-    <col customWidth="1" min="14" max="14" width="8.71"/>
-    <col customWidth="1" min="15" max="15" width="16.14"/>
-    <col customWidth="1" min="16" max="16" width="11.43"/>
-    <col customWidth="1" min="17" max="19" width="8.71"/>
+    <col customWidth="1" min="2" max="2" width="15.0"/>
+    <col customWidth="1" min="3" max="3" width="21.29"/>
+    <col customWidth="1" min="4" max="4" width="20.14"/>
+    <col customWidth="1" min="5" max="8" width="14.86"/>
+    <col customWidth="1" min="9" max="9" width="13.86"/>
+    <col customWidth="1" min="10" max="10" width="12.86"/>
+    <col customWidth="1" min="11" max="11" width="16.14"/>
+    <col customWidth="1" min="12" max="12" width="21.14"/>
+    <col customWidth="1" min="13" max="13" width="19.29"/>
+    <col customWidth="1" min="14" max="14" width="16.0"/>
+    <col customWidth="1" min="15" max="15" width="25.14"/>
+    <col customWidth="1" min="16" max="16" width="33.57"/>
+    <col customWidth="1" min="17" max="17" width="16.0"/>
+    <col customWidth="1" min="18" max="18" width="21.29"/>
+    <col customWidth="1" min="19" max="19" width="33.57"/>
+    <col customWidth="1" min="20" max="20" width="16.0"/>
+    <col customWidth="1" min="21" max="21" width="23.0"/>
+    <col customWidth="1" min="22" max="22" width="33.57"/>
   </cols>
   <sheetData>
     <row r="1">
@@ -489,7 +538,7 @@
       <c r="K1" s="1" t="s">
         <v>10</v>
       </c>
-      <c r="L1" s="2" t="s">
+      <c r="L1" s="1" t="s">
         <v>11</v>
       </c>
       <c r="M1" s="1" t="s">
@@ -504,143 +553,209 @@
       <c r="P1" s="1" t="s">
         <v>15</v>
       </c>
+      <c r="Q1" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="R1" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="S1" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="T1" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="U1" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="V1" s="1" t="s">
+        <v>15</v>
+      </c>
     </row>
     <row r="2">
-      <c r="C2" s="3">
-        <v>12.89</v>
-      </c>
-      <c r="D2" s="4" t="s">
+      <c r="A2" s="2" t="s">
         <v>16</v>
       </c>
-      <c r="E2" s="3" t="s">
+      <c r="B2" s="3" t="s">
         <v>17</v>
       </c>
-      <c r="F2" s="4" t="s">
+      <c r="C2" s="2" t="s">
         <v>18</v>
       </c>
+      <c r="D2" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="E2" s="3">
+        <v>1199.0</v>
+      </c>
+      <c r="F2" s="3">
+        <v>999.0</v>
+      </c>
       <c r="G2" s="3" t="s">
-        <v>19</v>
-      </c>
-      <c r="H2" s="3">
-        <v>23.0</v>
-      </c>
-      <c r="I2" s="3" t="s">
         <v>20</v>
       </c>
-      <c r="J2" s="3" t="s">
+      <c r="H2" s="3" t="s">
         <v>21</v>
       </c>
-      <c r="K2" s="3" t="s">
+      <c r="I2" s="2" t="s">
         <v>22</v>
       </c>
-      <c r="L2" s="3" t="s">
+      <c r="J2" s="2" t="s">
         <v>23</v>
       </c>
-      <c r="M2" s="3" t="s">
+      <c r="K2" s="2" t="s">
         <v>24</v>
       </c>
+      <c r="L2" s="2" t="s">
+        <v>25</v>
+      </c>
+      <c r="M2" s="2" t="s">
+        <v>26</v>
+      </c>
       <c r="N2" s="3" t="s">
-        <v>25</v>
+        <v>27</v>
       </c>
       <c r="O2" s="3" t="s">
-        <v>26</v>
+        <v>28</v>
       </c>
       <c r="P2" s="3" t="s">
-        <v>27</v>
-      </c>
+        <v>29</v>
+      </c>
+      <c r="Q2" s="3" t="s">
+        <v>30</v>
+      </c>
+      <c r="R2" s="3" t="s">
+        <v>31</v>
+      </c>
+      <c r="S2" s="3" t="s">
+        <v>29</v>
+      </c>
+      <c r="T2" s="3"/>
+      <c r="U2" s="3"/>
+      <c r="V2" s="3"/>
     </row>
     <row r="3">
-      <c r="A3" s="4" t="s">
-        <v>28</v>
-      </c>
-      <c r="B3" s="3">
-        <v>28.37</v>
-      </c>
-      <c r="C3" s="3">
-        <v>34.04</v>
-      </c>
-      <c r="D3" s="3" t="s">
-        <v>29</v>
-      </c>
-      <c r="E3" s="3" t="s">
-        <v>30</v>
-      </c>
-      <c r="F3" s="3" t="s">
-        <v>31</v>
+      <c r="A3" s="2" t="s">
+        <v>32</v>
+      </c>
+      <c r="B3" s="3" t="s">
+        <v>33</v>
+      </c>
+      <c r="C3" s="2" t="s">
+        <v>34</v>
+      </c>
+      <c r="D3" s="2" t="s">
+        <v>35</v>
+      </c>
+      <c r="E3" s="3">
+        <v>560.0</v>
+      </c>
+      <c r="F3" s="3">
+        <v>450.0</v>
       </c>
       <c r="G3" s="3" t="s">
-        <v>32</v>
-      </c>
-      <c r="H3" s="3">
-        <v>41.0</v>
-      </c>
-      <c r="I3" s="3" t="s">
-        <v>33</v>
-      </c>
-      <c r="J3" s="3" t="s">
-        <v>34</v>
-      </c>
-      <c r="K3" s="3" t="s">
-        <v>22</v>
-      </c>
-      <c r="L3" s="4" t="s">
-        <v>35</v>
-      </c>
-      <c r="M3" s="4" t="s">
         <v>36</v>
       </c>
+      <c r="H3" s="3" t="s">
+        <v>21</v>
+      </c>
+      <c r="I3" s="2" t="s">
+        <v>37</v>
+      </c>
+      <c r="J3" s="2" t="s">
+        <v>38</v>
+      </c>
+      <c r="K3" s="2" t="s">
+        <v>24</v>
+      </c>
+      <c r="L3" s="2" t="s">
+        <v>39</v>
+      </c>
+      <c r="M3" s="2" t="s">
+        <v>40</v>
+      </c>
       <c r="N3" s="3" t="s">
-        <v>37</v>
+        <v>41</v>
       </c>
       <c r="O3" s="3" t="s">
-        <v>26</v>
+        <v>42</v>
       </c>
       <c r="P3" s="3" t="s">
-        <v>38</v>
-      </c>
+        <v>43</v>
+      </c>
+      <c r="Q3" s="3"/>
+      <c r="R3" s="3"/>
+      <c r="S3" s="3"/>
+      <c r="T3" s="3"/>
+      <c r="U3" s="3"/>
+      <c r="V3" s="3"/>
     </row>
     <row r="4">
-      <c r="B4" s="3">
-        <v>20.18</v>
-      </c>
-      <c r="D4" s="3" t="s">
-        <v>29</v>
-      </c>
-      <c r="E4" s="3" t="s">
-        <v>39</v>
-      </c>
-      <c r="F4" s="4" t="s">
-        <v>40</v>
-      </c>
-      <c r="G4" s="3" t="s">
-        <v>41</v>
-      </c>
-      <c r="H4" s="3">
-        <v>61.0</v>
-      </c>
-      <c r="I4" s="3" t="s">
-        <v>42</v>
-      </c>
-      <c r="J4" s="3" t="s">
-        <v>43</v>
-      </c>
-      <c r="K4" s="3" t="s">
+      <c r="A4" s="2" t="s">
+        <v>44</v>
+      </c>
+      <c r="B4" s="3" t="s">
+        <v>45</v>
+      </c>
+      <c r="C4" s="2" t="s">
+        <v>34</v>
+      </c>
+      <c r="D4" s="2" t="s">
+        <v>46</v>
+      </c>
+      <c r="E4" s="3">
+        <v>1599.0</v>
+      </c>
+      <c r="F4" s="4">
+        <v>1300.0</v>
+      </c>
+      <c r="G4" s="4" t="s">
+        <v>47</v>
+      </c>
+      <c r="H4" s="4" t="s">
+        <v>48</v>
+      </c>
+      <c r="I4" s="2" t="s">
         <v>22</v>
       </c>
-      <c r="L4" s="4" t="s">
-        <v>35</v>
-      </c>
-      <c r="M4" s="3" t="s">
+      <c r="J4" s="2" t="s">
+        <v>49</v>
+      </c>
+      <c r="K4" s="2" t="s">
         <v>24</v>
       </c>
+      <c r="L4" s="2" t="s">
+        <v>50</v>
+      </c>
+      <c r="M4" s="2" t="s">
+        <v>51</v>
+      </c>
       <c r="N4" s="3" t="s">
-        <v>44</v>
+        <v>52</v>
       </c>
       <c r="O4" s="3" t="s">
-        <v>26</v>
+        <v>53</v>
       </c>
       <c r="P4" s="3" t="s">
-        <v>45</v>
+        <v>54</v>
+      </c>
+      <c r="Q4" s="3" t="s">
+        <v>55</v>
+      </c>
+      <c r="R4" s="3" t="s">
+        <v>56</v>
+      </c>
+      <c r="S4" s="3" t="s">
+        <v>54</v>
+      </c>
+      <c r="T4" s="3" t="s">
+        <v>57</v>
+      </c>
+      <c r="U4" s="3" t="s">
+        <v>58</v>
+      </c>
+      <c r="V4" s="3" t="s">
+        <v>54</v>
       </c>
     </row>
     <row r="5" ht="15.75" customHeight="1"/>
@@ -1617,6 +1732,28 @@
     <row r="976" ht="15.75" customHeight="1"/>
     <row r="977" ht="15.75" customHeight="1"/>
     <row r="978" ht="15.75" customHeight="1"/>
+    <row r="979" ht="15.75" customHeight="1"/>
+    <row r="980" ht="15.75" customHeight="1"/>
+    <row r="981" ht="15.75" customHeight="1"/>
+    <row r="982" ht="15.75" customHeight="1"/>
+    <row r="983" ht="15.75" customHeight="1"/>
+    <row r="984" ht="15.75" customHeight="1"/>
+    <row r="985" ht="15.75" customHeight="1"/>
+    <row r="986" ht="15.75" customHeight="1"/>
+    <row r="987" ht="15.75" customHeight="1"/>
+    <row r="988" ht="15.75" customHeight="1"/>
+    <row r="989" ht="15.75" customHeight="1"/>
+    <row r="990" ht="15.75" customHeight="1"/>
+    <row r="991" ht="15.75" customHeight="1"/>
+    <row r="992" ht="15.75" customHeight="1"/>
+    <row r="993" ht="15.75" customHeight="1"/>
+    <row r="994" ht="15.75" customHeight="1"/>
+    <row r="995" ht="15.75" customHeight="1"/>
+    <row r="996" ht="15.75" customHeight="1"/>
+    <row r="997" ht="15.75" customHeight="1"/>
+    <row r="998" ht="15.75" customHeight="1"/>
+    <row r="999" ht="15.75" customHeight="1"/>
+    <row r="1000" ht="15.75" customHeight="1"/>
   </sheetData>
   <printOptions/>
   <pageMargins bottom="1.0" footer="0.0" header="0.0" left="0.75" right="0.75" top="1.0"/>
@@ -1636,22 +1773,21 @@
   <sheetFormatPr customHeight="1" defaultColWidth="14.43" defaultRowHeight="15.0"/>
   <cols>
     <col customWidth="1" min="1" max="1" width="13.14"/>
-    <col customWidth="1" min="2" max="2" width="14.86"/>
-    <col customWidth="1" min="3" max="3" width="10.0"/>
-    <col customWidth="1" min="4" max="4" width="33.57"/>
-    <col customWidth="1" min="5" max="5" width="11.29"/>
-    <col customWidth="1" min="6" max="6" width="16.0"/>
-    <col customWidth="1" min="7" max="7" width="20.14"/>
-    <col customWidth="1" min="8" max="8" width="14.86"/>
-    <col customWidth="1" min="9" max="9" width="13.71"/>
-    <col customWidth="1" min="10" max="10" width="16.0"/>
-    <col customWidth="1" min="11" max="11" width="15.0"/>
-    <col customWidth="1" min="12" max="12" width="21.29"/>
-    <col customWidth="1" min="13" max="13" width="13.86"/>
-    <col customWidth="1" min="14" max="14" width="8.71"/>
-    <col customWidth="1" min="15" max="15" width="16.14"/>
-    <col customWidth="1" min="16" max="16" width="11.43"/>
-    <col customWidth="1" min="17" max="20" width="8.71"/>
+    <col customWidth="1" min="2" max="2" width="15.0"/>
+    <col customWidth="1" min="3" max="3" width="21.29"/>
+    <col customWidth="1" min="4" max="4" width="20.14"/>
+    <col customWidth="1" min="5" max="8" width="14.86"/>
+    <col customWidth="1" min="9" max="9" width="13.86"/>
+    <col customWidth="1" min="10" max="10" width="12.86"/>
+    <col customWidth="1" min="11" max="11" width="16.14"/>
+    <col customWidth="1" min="12" max="12" width="21.14"/>
+    <col customWidth="1" min="13" max="13" width="19.29"/>
+    <col customWidth="1" min="14" max="14" width="16.0"/>
+    <col customWidth="1" min="15" max="15" width="25.14"/>
+    <col customWidth="1" min="16" max="16" width="33.57"/>
+    <col customWidth="1" min="17" max="17" width="16.0"/>
+    <col customWidth="1" min="18" max="18" width="21.29"/>
+    <col customWidth="1" min="19" max="19" width="33.57"/>
   </cols>
   <sheetData>
     <row r="1">
@@ -1688,7 +1824,7 @@
       <c r="K1" s="1" t="s">
         <v>10</v>
       </c>
-      <c r="L1" s="2" t="s">
+      <c r="L1" s="1" t="s">
         <v>11</v>
       </c>
       <c r="M1" s="1" t="s">
@@ -1703,163 +1839,77 @@
       <c r="P1" s="1" t="s">
         <v>15</v>
       </c>
-      <c r="Q1" s="2" t="s">
-        <v>46</v>
+      <c r="Q1" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="R1" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="S1" s="1" t="s">
+        <v>15</v>
       </c>
     </row>
     <row r="2">
       <c r="A2" s="3" t="s">
-        <v>47</v>
-      </c>
-      <c r="B2" s="3">
-        <v>10.74</v>
-      </c>
-      <c r="C2" s="3">
-        <v>12.89</v>
-      </c>
-      <c r="D2" s="4" t="s">
-        <v>16</v>
-      </c>
-      <c r="E2" s="3" t="s">
-        <v>17</v>
-      </c>
-      <c r="F2" s="4" t="s">
-        <v>18</v>
+        <v>59</v>
+      </c>
+      <c r="B2" s="3" t="s">
+        <v>60</v>
+      </c>
+      <c r="C2" s="3" t="s">
+        <v>61</v>
+      </c>
+      <c r="D2" s="3" t="s">
+        <v>62</v>
+      </c>
+      <c r="E2" s="3">
+        <v>670.0</v>
+      </c>
+      <c r="F2" s="3">
+        <v>450.0</v>
       </c>
       <c r="G2" s="3" t="s">
-        <v>19</v>
-      </c>
-      <c r="H2" s="3">
-        <v>23.0</v>
+        <v>63</v>
+      </c>
+      <c r="H2" s="3" t="s">
+        <v>48</v>
       </c>
       <c r="I2" s="3" t="s">
-        <v>20</v>
-      </c>
-      <c r="J2" s="3" t="s">
-        <v>21</v>
-      </c>
-      <c r="K2" s="3" t="s">
-        <v>22</v>
-      </c>
-      <c r="L2" s="3" t="s">
+        <v>64</v>
+      </c>
+      <c r="J2" s="2" t="s">
         <v>23</v>
       </c>
-      <c r="M2" s="3" t="s">
+      <c r="K2" s="2" t="s">
         <v>24</v>
       </c>
+      <c r="L2" s="2" t="s">
+        <v>25</v>
+      </c>
+      <c r="M2" s="2" t="s">
+        <v>26</v>
+      </c>
       <c r="N2" s="3" t="s">
-        <v>25</v>
+        <v>27</v>
       </c>
       <c r="O2" s="3" t="s">
-        <v>26</v>
+        <v>28</v>
       </c>
       <c r="P2" s="3" t="s">
-        <v>27</v>
+        <v>29</v>
       </c>
       <c r="Q2" s="3" t="s">
-        <v>25</v>
+        <v>30</v>
+      </c>
+      <c r="R2" s="3" t="s">
+        <v>31</v>
+      </c>
+      <c r="S2" s="3" t="s">
+        <v>29</v>
       </c>
     </row>
-    <row r="3">
-      <c r="A3" s="3" t="s">
-        <v>48</v>
-      </c>
-      <c r="B3" s="3">
-        <v>28.37</v>
-      </c>
-      <c r="C3" s="3">
-        <v>34.04</v>
-      </c>
-      <c r="D3" s="3" t="s">
-        <v>29</v>
-      </c>
-      <c r="E3" s="3" t="s">
-        <v>30</v>
-      </c>
-      <c r="F3" s="3" t="s">
-        <v>31</v>
-      </c>
-      <c r="G3" s="3" t="s">
-        <v>32</v>
-      </c>
-      <c r="H3" s="3">
-        <v>41.0</v>
-      </c>
-      <c r="I3" s="3" t="s">
-        <v>33</v>
-      </c>
-      <c r="J3" s="3" t="s">
-        <v>34</v>
-      </c>
-      <c r="K3" s="3" t="s">
-        <v>22</v>
-      </c>
-      <c r="L3" s="4" t="s">
-        <v>35</v>
-      </c>
-      <c r="M3" s="4" t="s">
-        <v>36</v>
-      </c>
-      <c r="N3" s="3" t="s">
-        <v>37</v>
-      </c>
-      <c r="O3" s="3" t="s">
-        <v>26</v>
-      </c>
-      <c r="P3" s="3" t="s">
-        <v>38</v>
-      </c>
-    </row>
-    <row r="4">
-      <c r="A4" s="3" t="s">
-        <v>49</v>
-      </c>
-      <c r="B4" s="3">
-        <v>20.18</v>
-      </c>
-      <c r="D4" s="3" t="s">
-        <v>29</v>
-      </c>
-      <c r="E4" s="3" t="s">
-        <v>39</v>
-      </c>
-      <c r="F4" s="4" t="s">
-        <v>40</v>
-      </c>
-      <c r="G4" s="3" t="s">
-        <v>41</v>
-      </c>
-      <c r="H4" s="3">
-        <v>61.0</v>
-      </c>
-      <c r="I4" s="3" t="s">
-        <v>42</v>
-      </c>
-      <c r="J4" s="3" t="s">
-        <v>43</v>
-      </c>
-      <c r="K4" s="3" t="s">
-        <v>22</v>
-      </c>
-      <c r="L4" s="4" t="s">
-        <v>35</v>
-      </c>
-      <c r="M4" s="3" t="s">
-        <v>24</v>
-      </c>
-      <c r="N4" s="3" t="s">
-        <v>44</v>
-      </c>
-      <c r="O4" s="3" t="s">
-        <v>26</v>
-      </c>
-      <c r="P4" s="3" t="s">
-        <v>45</v>
-      </c>
-      <c r="Q4" s="3" t="s">
-        <v>50</v>
-      </c>
-    </row>
+    <row r="3" ht="15.75" customHeight="1"/>
+    <row r="4" ht="15.75" customHeight="1"/>
     <row r="5" ht="15.75" customHeight="1"/>
     <row r="6" ht="15.75" customHeight="1"/>
     <row r="7" ht="15.75" customHeight="1"/>
@@ -2834,6 +2884,26 @@
     <row r="976" ht="15.75" customHeight="1"/>
     <row r="977" ht="15.75" customHeight="1"/>
     <row r="978" ht="15.75" customHeight="1"/>
+    <row r="979" ht="15.75" customHeight="1"/>
+    <row r="980" ht="15.75" customHeight="1"/>
+    <row r="981" ht="15.75" customHeight="1"/>
+    <row r="982" ht="15.75" customHeight="1"/>
+    <row r="983" ht="15.75" customHeight="1"/>
+    <row r="984" ht="15.75" customHeight="1"/>
+    <row r="985" ht="15.75" customHeight="1"/>
+    <row r="986" ht="15.75" customHeight="1"/>
+    <row r="987" ht="15.75" customHeight="1"/>
+    <row r="988" ht="15.75" customHeight="1"/>
+    <row r="989" ht="15.75" customHeight="1"/>
+    <row r="990" ht="15.75" customHeight="1"/>
+    <row r="991" ht="15.75" customHeight="1"/>
+    <row r="992" ht="15.75" customHeight="1"/>
+    <row r="993" ht="15.75" customHeight="1"/>
+    <row r="994" ht="15.75" customHeight="1"/>
+    <row r="995" ht="15.75" customHeight="1"/>
+    <row r="996" ht="15.75" customHeight="1"/>
+    <row r="997" ht="15.75" customHeight="1"/>
+    <row r="998" ht="15.75" customHeight="1"/>
   </sheetData>
   <printOptions/>
   <pageMargins bottom="1.0" footer="0.0" header="0.0" left="0.75" right="0.75" top="1.0"/>

</xml_diff>